<commit_message>
Corrected LT1054 -5V power output label placement, identified which components are 0201 and corrected digi number and page of C-47,48,49,52,53,58 1u caps
</commit_message>
<xml_diff>
--- a/Documents/Music_Visualizer_BOM_Digikey_order.xlsx
+++ b/Documents/Music_Visualizer_BOM_Digikey_order.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B469F1BF-E824-41BD-A061-2B9A7BBBA0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5073413-BAE3-4113-AF86-99AA2AC838C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Music_Visualizer_BOM" sheetId="1" r:id="rId1"/>
+    <sheet name="Replacement parts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="298">
   <si>
     <t>Designator</t>
   </si>
@@ -852,13 +853,88 @@
   </si>
   <si>
     <t>SJ-3523-SMT-TR</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C21,C22,C37,C39,C40,C41,C42</t>
+  </si>
+  <si>
+    <t>587-GMK105CC6105KV-FTR-ND</t>
+  </si>
+  <si>
+    <t>GMK105CC6105KV-F</t>
+  </si>
+  <si>
+    <t>C60,C61</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>47nF</t>
+  </si>
+  <si>
+    <t>1.6nF</t>
+  </si>
+  <si>
+    <t>1nF</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>Case Code (mils)</t>
+  </si>
+  <si>
+    <t>0201</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>0402</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>45.3k</t>
+  </si>
+  <si>
+    <t>R58</t>
+  </si>
+  <si>
+    <t>48.7k</t>
+  </si>
+  <si>
+    <t>383k</t>
+  </si>
+  <si>
+    <t>22.6k</t>
+  </si>
+  <si>
+    <t>8.06k</t>
+  </si>
+  <si>
+    <t>R66,R67,R70</t>
+  </si>
+  <si>
+    <t>1k</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -989,6 +1065,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1335,8 +1417,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1696,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2998,4 +3081,299 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4868364-B3B3-4F6F-875E-7F5C634F5A51}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" t="s">
+        <v>277</v>
+      </c>
+      <c r="E5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>284</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" t="s">
+        <v>290</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E8" t="s">
+        <v>293</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" t="s">
+        <v>292</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" t="s">
+        <v>204</v>
+      </c>
+      <c r="E10" t="s">
+        <v>294</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>209</v>
+      </c>
+      <c r="D11" t="s">
+        <v>210</v>
+      </c>
+      <c r="E11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D12" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" t="s">
+        <v>297</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D13" t="s">
+        <v>240</v>
+      </c>
+      <c r="E13">
+        <v>330</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>